<commit_message>
fix invalid specialty and branch id format
</commit_message>
<xml_diff>
--- a/Book1.xlsx
+++ b/Book1.xlsx
@@ -831,7 +831,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="44">
+  <cellXfs count="43">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -873,63 +873,6 @@
     <xf numFmtId="165" fontId="1" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="165" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="165" fontId="1" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="165" fontId="1" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="165" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="165" fontId="1" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="165" fontId="1" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="164" fontId="1" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
@@ -958,6 +901,60 @@
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="165" fontId="1" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="1" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="1" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="1" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="1" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1274,10 +1271,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H135"/>
+  <dimension ref="A1:H134"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A118" workbookViewId="0">
-      <selection activeCell="D122" sqref="D122"/>
+    <sheetView tabSelected="1" topLeftCell="A133" workbookViewId="0">
+      <selection activeCell="K134" sqref="K134"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1286,10 +1283,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="20" t="s">
+      <c r="A1" s="27" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="20" t="s">
+      <c r="B1" s="27" t="s">
         <v>1</v>
       </c>
       <c r="C1" s="29" t="s">
@@ -1306,8 +1303,8 @@
       <c r="H1" s="33"/>
     </row>
     <row r="2" spans="1:8" ht="43.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="22"/>
-      <c r="B2" s="22"/>
+      <c r="A2" s="28"/>
+      <c r="B2" s="28"/>
       <c r="C2" s="30"/>
       <c r="D2" s="30"/>
       <c r="E2" s="1" t="s">
@@ -1322,7 +1319,7 @@
       </c>
     </row>
     <row r="3" spans="1:8" ht="171.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="20">
+      <c r="A3" s="27">
         <v>1</v>
       </c>
       <c r="B3" s="12" t="s">
@@ -1337,16 +1334,16 @@
       <c r="E3" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="F3" s="18" t="s">
+      <c r="F3" s="25" t="s">
         <v>11</v>
       </c>
-      <c r="G3" s="19"/>
+      <c r="G3" s="26"/>
       <c r="H3" s="3" t="s">
         <v>178</v>
       </c>
     </row>
     <row r="4" spans="1:8" ht="171.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="21"/>
+      <c r="A4" s="39"/>
       <c r="B4" s="13"/>
       <c r="C4" s="11">
         <v>13</v>
@@ -1357,16 +1354,16 @@
       <c r="E4" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="F4" s="18" t="s">
-        <v>13</v>
-      </c>
-      <c r="G4" s="19"/>
+      <c r="F4" s="25" t="s">
+        <v>13</v>
+      </c>
+      <c r="G4" s="26"/>
       <c r="H4" s="3" t="s">
         <v>182</v>
       </c>
     </row>
     <row r="5" spans="1:8" ht="114.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="21"/>
+      <c r="A5" s="39"/>
       <c r="B5" s="13"/>
       <c r="C5" s="11">
         <v>14</v>
@@ -1375,12 +1372,12 @@
         <v>14</v>
       </c>
       <c r="E5" s="6"/>
-      <c r="F5" s="15"/>
-      <c r="G5" s="17"/>
+      <c r="F5" s="40"/>
+      <c r="G5" s="41"/>
       <c r="H5" s="2"/>
     </row>
     <row r="6" spans="1:8" ht="171.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="21"/>
+      <c r="A6" s="39"/>
       <c r="B6" s="13"/>
       <c r="C6" s="11" t="s">
         <v>15</v>
@@ -1391,16 +1388,16 @@
       <c r="E6" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="F6" s="18" t="s">
+      <c r="F6" s="25" t="s">
         <v>11</v>
       </c>
-      <c r="G6" s="19"/>
+      <c r="G6" s="26"/>
       <c r="H6" s="3" t="s">
         <v>178</v>
       </c>
     </row>
     <row r="7" spans="1:8" ht="171.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="21"/>
+      <c r="A7" s="39"/>
       <c r="B7" s="13"/>
       <c r="C7" s="11" t="s">
         <v>17</v>
@@ -1411,16 +1408,16 @@
       <c r="E7" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="F7" s="18" t="s">
+      <c r="F7" s="25" t="s">
         <v>19</v>
       </c>
-      <c r="G7" s="19"/>
+      <c r="G7" s="26"/>
       <c r="H7" s="3" t="s">
         <v>183</v>
       </c>
     </row>
     <row r="8" spans="1:8" ht="171.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="21"/>
+      <c r="A8" s="39"/>
       <c r="B8" s="13"/>
       <c r="C8" s="11" t="s">
         <v>20</v>
@@ -1431,16 +1428,16 @@
       <c r="E8" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="F8" s="18" t="s">
+      <c r="F8" s="25" t="s">
         <v>11</v>
       </c>
-      <c r="G8" s="19"/>
+      <c r="G8" s="26"/>
       <c r="H8" s="3" t="s">
         <v>178</v>
       </c>
     </row>
     <row r="9" spans="1:8" ht="171.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="21"/>
+      <c r="A9" s="39"/>
       <c r="B9" s="13"/>
       <c r="C9" s="11" t="s">
         <v>22</v>
@@ -1451,16 +1448,16 @@
       <c r="E9" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="F9" s="18" t="s">
-        <v>13</v>
-      </c>
-      <c r="G9" s="19"/>
+      <c r="F9" s="25" t="s">
+        <v>13</v>
+      </c>
+      <c r="G9" s="26"/>
       <c r="H9" s="3" t="s">
         <v>182</v>
       </c>
     </row>
     <row r="10" spans="1:8" ht="186" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="21"/>
+      <c r="A10" s="39"/>
       <c r="B10" s="13"/>
       <c r="C10" s="11" t="s">
         <v>25</v>
@@ -1471,16 +1468,16 @@
       <c r="E10" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="F10" s="18" t="s">
+      <c r="F10" s="25" t="s">
         <v>27</v>
       </c>
-      <c r="G10" s="19"/>
+      <c r="G10" s="26"/>
       <c r="H10" s="3" t="s">
         <v>184</v>
       </c>
     </row>
     <row r="11" spans="1:8" ht="200.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="21"/>
+      <c r="A11" s="39"/>
       <c r="B11" s="13"/>
       <c r="C11" s="11" t="s">
         <v>28</v>
@@ -1491,16 +1488,16 @@
       <c r="E11" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="F11" s="18" t="s">
+      <c r="F11" s="25" t="s">
         <v>30</v>
       </c>
-      <c r="G11" s="19"/>
+      <c r="G11" s="26"/>
       <c r="H11" s="3" t="s">
         <v>185</v>
       </c>
     </row>
     <row r="12" spans="1:8" ht="186" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="21"/>
+      <c r="A12" s="39"/>
       <c r="B12" s="13"/>
       <c r="C12" s="11" t="s">
         <v>31</v>
@@ -1511,16 +1508,16 @@
       <c r="E12" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="F12" s="18" t="s">
+      <c r="F12" s="25" t="s">
         <v>33</v>
       </c>
-      <c r="G12" s="19"/>
+      <c r="G12" s="26"/>
       <c r="H12" s="3" t="s">
         <v>186</v>
       </c>
     </row>
     <row r="13" spans="1:8" ht="171.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="21"/>
+      <c r="A13" s="39"/>
       <c r="B13" s="13"/>
       <c r="C13" s="11" t="s">
         <v>34</v>
@@ -1531,16 +1528,16 @@
       <c r="E13" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="F13" s="18" t="s">
-        <v>13</v>
-      </c>
-      <c r="G13" s="19"/>
+      <c r="F13" s="25" t="s">
+        <v>13</v>
+      </c>
+      <c r="G13" s="26"/>
       <c r="H13" s="3" t="s">
         <v>182</v>
       </c>
     </row>
     <row r="14" spans="1:8" ht="171.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="22"/>
+      <c r="A14" s="28"/>
       <c r="B14" s="14"/>
       <c r="C14" s="11" t="s">
         <v>36</v>
@@ -1551,17 +1548,17 @@
       <c r="E14" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="F14" s="18" t="s">
-        <v>13</v>
-      </c>
-      <c r="G14" s="19"/>
+      <c r="F14" s="25" t="s">
+        <v>13</v>
+      </c>
+      <c r="G14" s="26"/>
       <c r="H14" s="3" t="s">
         <v>182</v>
       </c>
     </row>
     <row r="15" spans="1:8" ht="171.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="26"/>
-      <c r="B15" s="26"/>
+      <c r="A15" s="36"/>
+      <c r="B15" s="36"/>
       <c r="C15" s="11" t="s">
         <v>38</v>
       </c>
@@ -1571,17 +1568,17 @@
       <c r="E15" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="F15" s="18" t="s">
-        <v>13</v>
-      </c>
-      <c r="G15" s="19"/>
+      <c r="F15" s="25" t="s">
+        <v>13</v>
+      </c>
+      <c r="G15" s="26"/>
       <c r="H15" s="3" t="s">
         <v>182</v>
       </c>
     </row>
     <row r="16" spans="1:8" ht="186" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="27"/>
-      <c r="B16" s="27"/>
+      <c r="A16" s="37"/>
+      <c r="B16" s="37"/>
       <c r="C16" s="11" t="s">
         <v>40</v>
       </c>
@@ -1591,17 +1588,17 @@
       <c r="E16" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="F16" s="18" t="s">
+      <c r="F16" s="25" t="s">
         <v>27</v>
       </c>
-      <c r="G16" s="19"/>
+      <c r="G16" s="26"/>
       <c r="H16" s="3" t="s">
         <v>184</v>
       </c>
     </row>
     <row r="17" spans="1:8" ht="171.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="27"/>
-      <c r="B17" s="27"/>
+      <c r="A17" s="37"/>
+      <c r="B17" s="37"/>
       <c r="C17" s="11" t="s">
         <v>42</v>
       </c>
@@ -1611,17 +1608,17 @@
       <c r="E17" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="F17" s="18" t="s">
+      <c r="F17" s="25" t="s">
         <v>11</v>
       </c>
-      <c r="G17" s="19"/>
+      <c r="G17" s="26"/>
       <c r="H17" s="3" t="s">
         <v>178</v>
       </c>
     </row>
     <row r="18" spans="1:8" ht="171.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="27"/>
-      <c r="B18" s="27"/>
+      <c r="A18" s="37"/>
+      <c r="B18" s="37"/>
       <c r="C18" s="11" t="s">
         <v>44</v>
       </c>
@@ -1631,17 +1628,17 @@
       <c r="E18" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="F18" s="18" t="s">
+      <c r="F18" s="25" t="s">
         <v>11</v>
       </c>
-      <c r="G18" s="19"/>
+      <c r="G18" s="26"/>
       <c r="H18" s="3" t="s">
         <v>178</v>
       </c>
     </row>
     <row r="19" spans="1:8" ht="186" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="27"/>
-      <c r="B19" s="27"/>
+      <c r="A19" s="37"/>
+      <c r="B19" s="37"/>
       <c r="C19" s="11" t="s">
         <v>46</v>
       </c>
@@ -1651,17 +1648,17 @@
       <c r="E19" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="F19" s="18" t="s">
+      <c r="F19" s="25" t="s">
         <v>27</v>
       </c>
-      <c r="G19" s="19"/>
+      <c r="G19" s="26"/>
       <c r="H19" s="3" t="s">
         <v>184</v>
       </c>
     </row>
     <row r="20" spans="1:8" ht="171.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="27"/>
-      <c r="B20" s="27"/>
+      <c r="A20" s="37"/>
+      <c r="B20" s="37"/>
       <c r="C20" s="11">
         <v>15</v>
       </c>
@@ -1671,17 +1668,17 @@
       <c r="E20" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="F20" s="18" t="s">
-        <v>13</v>
-      </c>
-      <c r="G20" s="19"/>
+      <c r="F20" s="25" t="s">
+        <v>13</v>
+      </c>
+      <c r="G20" s="26"/>
       <c r="H20" s="3" t="s">
         <v>182</v>
       </c>
     </row>
     <row r="21" spans="1:8" ht="186" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="27"/>
-      <c r="B21" s="27"/>
+      <c r="A21" s="37"/>
+      <c r="B21" s="37"/>
       <c r="C21" s="11">
         <v>16</v>
       </c>
@@ -1691,17 +1688,17 @@
       <c r="E21" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="F21" s="18" t="s">
+      <c r="F21" s="25" t="s">
         <v>27</v>
       </c>
-      <c r="G21" s="19"/>
+      <c r="G21" s="26"/>
       <c r="H21" s="3" t="s">
         <v>184</v>
       </c>
     </row>
     <row r="22" spans="1:8" ht="57.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="28"/>
-      <c r="B22" s="28"/>
+      <c r="A22" s="38"/>
+      <c r="B22" s="38"/>
       <c r="C22" s="11">
         <v>17</v>
       </c>
@@ -1711,19 +1708,19 @@
       <c r="E22" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="F22" s="18" t="s">
+      <c r="F22" s="25" t="s">
         <v>27</v>
       </c>
-      <c r="G22" s="19"/>
+      <c r="G22" s="26"/>
       <c r="H22" s="3" t="s">
         <v>51</v>
       </c>
     </row>
     <row r="23" spans="1:8" ht="86.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="20">
+      <c r="A23" s="27">
         <v>2</v>
       </c>
-      <c r="B23" s="23" t="s">
+      <c r="B23" s="34" t="s">
         <v>52</v>
       </c>
       <c r="C23" s="11">
@@ -1735,17 +1732,17 @@
       <c r="E23" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="F23" s="18" t="s">
+      <c r="F23" s="25" t="s">
         <v>54</v>
       </c>
-      <c r="G23" s="19"/>
+      <c r="G23" s="26"/>
       <c r="H23" s="3" t="s">
         <v>51</v>
       </c>
     </row>
     <row r="24" spans="1:8" ht="257.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A24" s="22"/>
-      <c r="B24" s="25"/>
+      <c r="A24" s="28"/>
+      <c r="B24" s="35"/>
       <c r="C24" s="11">
         <v>22</v>
       </c>
@@ -1755,17 +1752,17 @@
       <c r="E24" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="F24" s="18" t="s">
-        <v>13</v>
-      </c>
-      <c r="G24" s="19"/>
+      <c r="F24" s="25" t="s">
+        <v>13</v>
+      </c>
+      <c r="G24" s="26"/>
       <c r="H24" s="3" t="s">
         <v>51</v>
       </c>
     </row>
     <row r="25" spans="1:8" ht="257.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A25" s="26"/>
-      <c r="B25" s="26"/>
+      <c r="A25" s="36"/>
+      <c r="B25" s="36"/>
       <c r="C25" s="11">
         <v>22</v>
       </c>
@@ -1775,17 +1772,17 @@
       <c r="E25" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="F25" s="18" t="s">
-        <v>13</v>
-      </c>
-      <c r="G25" s="19"/>
+      <c r="F25" s="25" t="s">
+        <v>13</v>
+      </c>
+      <c r="G25" s="26"/>
       <c r="H25" s="3" t="s">
         <v>182</v>
       </c>
     </row>
     <row r="26" spans="1:8" ht="143.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A26" s="27"/>
-      <c r="B26" s="27"/>
+      <c r="A26" s="37"/>
+      <c r="B26" s="37"/>
       <c r="C26" s="11">
         <v>23</v>
       </c>
@@ -1795,17 +1792,17 @@
       <c r="E26" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="F26" s="18" t="s">
+      <c r="F26" s="25" t="s">
         <v>55</v>
       </c>
-      <c r="G26" s="19"/>
+      <c r="G26" s="26"/>
       <c r="H26" s="3" t="s">
         <v>51</v>
       </c>
     </row>
     <row r="27" spans="1:8" ht="72" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A27" s="27"/>
-      <c r="B27" s="27"/>
+      <c r="A27" s="37"/>
+      <c r="B27" s="37"/>
       <c r="C27" s="11">
         <v>24</v>
       </c>
@@ -1815,17 +1812,17 @@
       <c r="E27" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="F27" s="18" t="s">
+      <c r="F27" s="25" t="s">
         <v>57</v>
       </c>
-      <c r="G27" s="19"/>
+      <c r="G27" s="26"/>
       <c r="H27" s="3" t="s">
         <v>51</v>
       </c>
     </row>
     <row r="28" spans="1:8" ht="72" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A28" s="27"/>
-      <c r="B28" s="27"/>
+      <c r="A28" s="37"/>
+      <c r="B28" s="37"/>
       <c r="C28" s="11">
         <v>25</v>
       </c>
@@ -1835,17 +1832,17 @@
       <c r="E28" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="F28" s="18" t="s">
+      <c r="F28" s="25" t="s">
         <v>190</v>
       </c>
-      <c r="G28" s="19"/>
+      <c r="G28" s="26"/>
       <c r="H28" s="3" t="s">
         <v>51</v>
       </c>
     </row>
     <row r="29" spans="1:8" ht="72" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A29" s="27"/>
-      <c r="B29" s="27"/>
+      <c r="A29" s="37"/>
+      <c r="B29" s="37"/>
       <c r="C29" s="11">
         <v>26</v>
       </c>
@@ -1855,17 +1852,17 @@
       <c r="E29" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="F29" s="18" t="s">
+      <c r="F29" s="25" t="s">
         <v>60</v>
       </c>
-      <c r="G29" s="19"/>
+      <c r="G29" s="26"/>
       <c r="H29" s="3" t="s">
         <v>51</v>
       </c>
     </row>
     <row r="30" spans="1:8" ht="171.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A30" s="27"/>
-      <c r="B30" s="27"/>
+      <c r="A30" s="37"/>
+      <c r="B30" s="37"/>
       <c r="C30" s="11">
         <v>27</v>
       </c>
@@ -1875,17 +1872,17 @@
       <c r="E30" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="F30" s="18" t="s">
+      <c r="F30" s="25" t="s">
         <v>11</v>
       </c>
-      <c r="G30" s="19"/>
+      <c r="G30" s="26"/>
       <c r="H30" s="3" t="s">
         <v>178</v>
       </c>
     </row>
     <row r="31" spans="1:8" ht="171.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A31" s="27"/>
-      <c r="B31" s="27"/>
+      <c r="A31" s="37"/>
+      <c r="B31" s="37"/>
       <c r="C31" s="11">
         <v>28</v>
       </c>
@@ -1895,17 +1892,17 @@
       <c r="E31" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="F31" s="18" t="s">
-        <v>13</v>
-      </c>
-      <c r="G31" s="19"/>
+      <c r="F31" s="25" t="s">
+        <v>13</v>
+      </c>
+      <c r="G31" s="26"/>
       <c r="H31" s="3" t="s">
         <v>182</v>
       </c>
     </row>
     <row r="32" spans="1:8" ht="171.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A32" s="28"/>
-      <c r="B32" s="28"/>
+      <c r="A32" s="38"/>
+      <c r="B32" s="38"/>
       <c r="C32" s="11">
         <v>29</v>
       </c>
@@ -1915,19 +1912,19 @@
       <c r="E32" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="F32" s="18" t="s">
+      <c r="F32" s="25" t="s">
         <v>11</v>
       </c>
-      <c r="G32" s="19"/>
+      <c r="G32" s="26"/>
       <c r="H32" s="3" t="s">
         <v>178</v>
       </c>
     </row>
     <row r="33" spans="1:8" ht="171.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A33" s="20">
+      <c r="A33" s="27">
         <v>3</v>
       </c>
-      <c r="B33" s="23" t="s">
+      <c r="B33" s="34" t="s">
         <v>62</v>
       </c>
       <c r="C33" s="11">
@@ -1939,17 +1936,17 @@
       <c r="E33" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="F33" s="18" t="s">
+      <c r="F33" s="25" t="s">
         <v>11</v>
       </c>
-      <c r="G33" s="19"/>
+      <c r="G33" s="26"/>
       <c r="H33" s="3" t="s">
         <v>178</v>
       </c>
     </row>
     <row r="34" spans="1:8" ht="171.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A34" s="21"/>
-      <c r="B34" s="24"/>
+      <c r="A34" s="39"/>
+      <c r="B34" s="42"/>
       <c r="C34" s="11">
         <v>32</v>
       </c>
@@ -1959,17 +1956,17 @@
       <c r="E34" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="F34" s="18" t="s">
+      <c r="F34" s="25" t="s">
         <v>11</v>
       </c>
-      <c r="G34" s="19"/>
+      <c r="G34" s="26"/>
       <c r="H34" s="3" t="s">
         <v>178</v>
       </c>
     </row>
     <row r="35" spans="1:8" ht="171.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A35" s="21"/>
-      <c r="B35" s="24"/>
+      <c r="A35" s="39"/>
+      <c r="B35" s="42"/>
       <c r="C35" s="11">
         <v>33</v>
       </c>
@@ -1979,17 +1976,17 @@
       <c r="E35" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="F35" s="18" t="s">
+      <c r="F35" s="25" t="s">
         <v>11</v>
       </c>
-      <c r="G35" s="19"/>
+      <c r="G35" s="26"/>
       <c r="H35" s="3" t="s">
         <v>178</v>
       </c>
     </row>
     <row r="36" spans="1:8" ht="171.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A36" s="21"/>
-      <c r="B36" s="24"/>
+      <c r="A36" s="39"/>
+      <c r="B36" s="42"/>
       <c r="C36" s="11">
         <v>34</v>
       </c>
@@ -1999,17 +1996,17 @@
       <c r="E36" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="F36" s="18" t="s">
+      <c r="F36" s="25" t="s">
         <v>11</v>
       </c>
-      <c r="G36" s="19"/>
+      <c r="G36" s="26"/>
       <c r="H36" s="3" t="s">
         <v>178</v>
       </c>
     </row>
     <row r="37" spans="1:8" ht="171.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A37" s="22"/>
-      <c r="B37" s="25"/>
+      <c r="A37" s="28"/>
+      <c r="B37" s="35"/>
       <c r="C37" s="11">
         <v>35</v>
       </c>
@@ -2019,19 +2016,19 @@
       <c r="E37" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="F37" s="18" t="s">
+      <c r="F37" s="25" t="s">
         <v>19</v>
       </c>
-      <c r="G37" s="19"/>
+      <c r="G37" s="26"/>
       <c r="H37" s="3" t="s">
         <v>183</v>
       </c>
     </row>
     <row r="38" spans="1:8" ht="171.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A38" s="20">
+      <c r="A38" s="27">
         <v>5</v>
       </c>
-      <c r="B38" s="23" t="s">
+      <c r="B38" s="34" t="s">
         <v>68</v>
       </c>
       <c r="C38" s="11">
@@ -2043,17 +2040,17 @@
       <c r="E38" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="F38" s="18" t="s">
-        <v>13</v>
-      </c>
-      <c r="G38" s="19"/>
+      <c r="F38" s="25" t="s">
+        <v>13</v>
+      </c>
+      <c r="G38" s="26"/>
       <c r="H38" s="3" t="s">
         <v>182</v>
       </c>
     </row>
     <row r="39" spans="1:8" ht="171.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A39" s="21"/>
-      <c r="B39" s="24"/>
+      <c r="A39" s="39"/>
+      <c r="B39" s="42"/>
       <c r="C39" s="11">
         <v>52</v>
       </c>
@@ -2063,17 +2060,17 @@
       <c r="E39" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="F39" s="18" t="s">
+      <c r="F39" s="25" t="s">
         <v>71</v>
       </c>
-      <c r="G39" s="19"/>
+      <c r="G39" s="26"/>
       <c r="H39" s="3" t="s">
         <v>182</v>
       </c>
     </row>
     <row r="40" spans="1:8" ht="171.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A40" s="21"/>
-      <c r="B40" s="24"/>
+      <c r="A40" s="39"/>
+      <c r="B40" s="42"/>
       <c r="C40" s="11">
         <v>53</v>
       </c>
@@ -2083,17 +2080,17 @@
       <c r="E40" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="F40" s="18" t="s">
-        <v>13</v>
-      </c>
-      <c r="G40" s="19"/>
+      <c r="F40" s="25" t="s">
+        <v>13</v>
+      </c>
+      <c r="G40" s="26"/>
       <c r="H40" s="3" t="s">
         <v>182</v>
       </c>
     </row>
     <row r="41" spans="1:8" ht="171.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A41" s="22"/>
-      <c r="B41" s="25"/>
+      <c r="A41" s="28"/>
+      <c r="B41" s="35"/>
       <c r="C41" s="11">
         <v>54</v>
       </c>
@@ -2103,10 +2100,10 @@
       <c r="E41" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="F41" s="18" t="s">
-        <v>13</v>
-      </c>
-      <c r="G41" s="19"/>
+      <c r="F41" s="25" t="s">
+        <v>13</v>
+      </c>
+      <c r="G41" s="26"/>
       <c r="H41" s="3" t="s">
         <v>182</v>
       </c>
@@ -2127,19 +2124,19 @@
       <c r="E42" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="F42" s="18" t="s">
-        <v>13</v>
-      </c>
-      <c r="G42" s="19"/>
+      <c r="F42" s="25" t="s">
+        <v>13</v>
+      </c>
+      <c r="G42" s="26"/>
       <c r="H42" s="3" t="s">
         <v>193</v>
       </c>
     </row>
     <row r="43" spans="1:8" ht="171.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A43" s="20">
+      <c r="A43" s="27">
         <v>7</v>
       </c>
-      <c r="B43" s="23" t="s">
+      <c r="B43" s="34" t="s">
         <v>75</v>
       </c>
       <c r="C43" s="11">
@@ -2151,17 +2148,17 @@
       <c r="E43" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="F43" s="18" t="s">
-        <v>13</v>
-      </c>
-      <c r="G43" s="19"/>
+      <c r="F43" s="25" t="s">
+        <v>13</v>
+      </c>
+      <c r="G43" s="26"/>
       <c r="H43" s="3" t="s">
         <v>182</v>
       </c>
     </row>
     <row r="44" spans="1:8" ht="171.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A44" s="21"/>
-      <c r="B44" s="24"/>
+      <c r="A44" s="39"/>
+      <c r="B44" s="42"/>
       <c r="C44" s="11">
         <v>72</v>
       </c>
@@ -2171,17 +2168,17 @@
       <c r="E44" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="F44" s="18" t="s">
-        <v>13</v>
-      </c>
-      <c r="G44" s="19"/>
+      <c r="F44" s="25" t="s">
+        <v>13</v>
+      </c>
+      <c r="G44" s="26"/>
       <c r="H44" s="3" t="s">
         <v>182</v>
       </c>
     </row>
     <row r="45" spans="1:8" ht="171.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A45" s="21"/>
-      <c r="B45" s="24"/>
+      <c r="A45" s="39"/>
+      <c r="B45" s="42"/>
       <c r="C45" s="11">
         <v>73</v>
       </c>
@@ -2191,17 +2188,17 @@
       <c r="E45" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="F45" s="18" t="s">
-        <v>13</v>
-      </c>
-      <c r="G45" s="19"/>
+      <c r="F45" s="25" t="s">
+        <v>13</v>
+      </c>
+      <c r="G45" s="26"/>
       <c r="H45" s="3" t="s">
         <v>182</v>
       </c>
     </row>
     <row r="46" spans="1:8" ht="171.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A46" s="21"/>
-      <c r="B46" s="24"/>
+      <c r="A46" s="39"/>
+      <c r="B46" s="42"/>
       <c r="C46" s="11">
         <v>75</v>
       </c>
@@ -2211,17 +2208,17 @@
       <c r="E46" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="F46" s="18" t="s">
-        <v>13</v>
-      </c>
-      <c r="G46" s="19"/>
+      <c r="F46" s="25" t="s">
+        <v>13</v>
+      </c>
+      <c r="G46" s="26"/>
       <c r="H46" s="3" t="s">
         <v>182</v>
       </c>
     </row>
     <row r="47" spans="1:8" ht="171.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A47" s="22"/>
-      <c r="B47" s="25"/>
+      <c r="A47" s="28"/>
+      <c r="B47" s="35"/>
       <c r="C47" s="11">
         <v>76</v>
       </c>
@@ -2231,10 +2228,10 @@
       <c r="E47" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="F47" s="18" t="s">
-        <v>13</v>
-      </c>
-      <c r="G47" s="19"/>
+      <c r="F47" s="25" t="s">
+        <v>13</v>
+      </c>
+      <c r="G47" s="26"/>
       <c r="H47" s="3" t="s">
         <v>182</v>
       </c>
@@ -2255,10 +2252,10 @@
       <c r="E48" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="F48" s="18" t="s">
+      <c r="F48" s="25" t="s">
         <v>11</v>
       </c>
-      <c r="G48" s="19"/>
+      <c r="G48" s="26"/>
       <c r="H48" s="3" t="s">
         <v>80</v>
       </c>
@@ -2279,19 +2276,19 @@
       <c r="E49" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="F49" s="18" t="s">
+      <c r="F49" s="25" t="s">
         <v>27</v>
       </c>
-      <c r="G49" s="19"/>
+      <c r="G49" s="26"/>
       <c r="H49" s="3" t="s">
         <v>184</v>
       </c>
     </row>
     <row r="50" spans="1:8" ht="186" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A50" s="20">
-        <v>10</v>
-      </c>
-      <c r="B50" s="23" t="s">
+      <c r="A50" s="27">
+        <v>10</v>
+      </c>
+      <c r="B50" s="34" t="s">
         <v>82</v>
       </c>
       <c r="C50" s="11">
@@ -2303,17 +2300,17 @@
       <c r="E50" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="F50" s="18" t="s">
+      <c r="F50" s="25" t="s">
         <v>27</v>
       </c>
-      <c r="G50" s="19"/>
+      <c r="G50" s="26"/>
       <c r="H50" s="3" t="s">
         <v>184</v>
       </c>
     </row>
     <row r="51" spans="1:8" ht="200.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A51" s="21"/>
-      <c r="B51" s="24"/>
+      <c r="A51" s="39"/>
+      <c r="B51" s="42"/>
       <c r="C51" s="11">
         <v>102</v>
       </c>
@@ -2323,17 +2320,17 @@
       <c r="E51" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="F51" s="18" t="s">
+      <c r="F51" s="25" t="s">
         <v>30</v>
       </c>
-      <c r="G51" s="19"/>
+      <c r="G51" s="26"/>
       <c r="H51" s="3" t="s">
         <v>185</v>
       </c>
     </row>
     <row r="52" spans="1:8" ht="171.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A52" s="21"/>
-      <c r="B52" s="24"/>
+      <c r="A52" s="39"/>
+      <c r="B52" s="42"/>
       <c r="C52" s="11">
         <v>103</v>
       </c>
@@ -2343,17 +2340,17 @@
       <c r="E52" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="F52" s="18" t="s">
-        <v>13</v>
-      </c>
-      <c r="G52" s="19"/>
+      <c r="F52" s="25" t="s">
+        <v>13</v>
+      </c>
+      <c r="G52" s="26"/>
       <c r="H52" s="3" t="s">
         <v>182</v>
       </c>
     </row>
     <row r="53" spans="1:8" ht="171.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A53" s="21"/>
-      <c r="B53" s="24"/>
+      <c r="A53" s="39"/>
+      <c r="B53" s="42"/>
       <c r="C53" s="11">
         <v>104</v>
       </c>
@@ -2363,17 +2360,17 @@
       <c r="E53" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="F53" s="18" t="s">
-        <v>13</v>
-      </c>
-      <c r="G53" s="19"/>
+      <c r="F53" s="25" t="s">
+        <v>13</v>
+      </c>
+      <c r="G53" s="26"/>
       <c r="H53" s="3" t="s">
         <v>182</v>
       </c>
     </row>
     <row r="54" spans="1:8" ht="171.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A54" s="21"/>
-      <c r="B54" s="24"/>
+      <c r="A54" s="39"/>
+      <c r="B54" s="42"/>
       <c r="C54" s="11">
         <v>105</v>
       </c>
@@ -2383,17 +2380,17 @@
       <c r="E54" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="F54" s="18" t="s">
-        <v>13</v>
-      </c>
-      <c r="G54" s="19"/>
+      <c r="F54" s="25" t="s">
+        <v>13</v>
+      </c>
+      <c r="G54" s="26"/>
       <c r="H54" s="3" t="s">
         <v>182</v>
       </c>
     </row>
     <row r="55" spans="1:8" ht="186" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A55" s="22"/>
-      <c r="B55" s="25"/>
+      <c r="A55" s="28"/>
+      <c r="B55" s="35"/>
       <c r="C55" s="11">
         <v>106</v>
       </c>
@@ -2403,19 +2400,19 @@
       <c r="E55" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="F55" s="18" t="s">
+      <c r="F55" s="25" t="s">
         <v>33</v>
       </c>
-      <c r="G55" s="19"/>
+      <c r="G55" s="26"/>
       <c r="H55" s="3" t="s">
         <v>186</v>
       </c>
     </row>
     <row r="56" spans="1:8" ht="171.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A56" s="20">
+      <c r="A56" s="27">
         <v>11</v>
       </c>
-      <c r="B56" s="23" t="s">
+      <c r="B56" s="34" t="s">
         <v>89</v>
       </c>
       <c r="C56" s="11">
@@ -2427,17 +2424,17 @@
       <c r="E56" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="F56" s="18" t="s">
-        <v>13</v>
-      </c>
-      <c r="G56" s="19"/>
+      <c r="F56" s="25" t="s">
+        <v>13</v>
+      </c>
+      <c r="G56" s="26"/>
       <c r="H56" s="3" t="s">
         <v>182</v>
       </c>
     </row>
     <row r="57" spans="1:8" ht="171.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A57" s="21"/>
-      <c r="B57" s="24"/>
+      <c r="A57" s="39"/>
+      <c r="B57" s="42"/>
       <c r="C57" s="11">
         <v>112</v>
       </c>
@@ -2447,17 +2444,17 @@
       <c r="E57" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="F57" s="18" t="s">
-        <v>13</v>
-      </c>
-      <c r="G57" s="19"/>
+      <c r="F57" s="25" t="s">
+        <v>13</v>
+      </c>
+      <c r="G57" s="26"/>
       <c r="H57" s="3" t="s">
         <v>182</v>
       </c>
     </row>
     <row r="58" spans="1:8" ht="171.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A58" s="22"/>
-      <c r="B58" s="25"/>
+      <c r="A58" s="28"/>
+      <c r="B58" s="35"/>
       <c r="C58" s="11">
         <v>113</v>
       </c>
@@ -2467,19 +2464,19 @@
       <c r="E58" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="F58" s="18" t="s">
-        <v>13</v>
-      </c>
-      <c r="G58" s="19"/>
+      <c r="F58" s="25" t="s">
+        <v>13</v>
+      </c>
+      <c r="G58" s="26"/>
       <c r="H58" s="3" t="s">
         <v>182</v>
       </c>
     </row>
     <row r="59" spans="1:8" ht="171.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A59" s="20">
+      <c r="A59" s="27">
         <v>12</v>
       </c>
-      <c r="B59" s="23" t="s">
+      <c r="B59" s="34" t="s">
         <v>93</v>
       </c>
       <c r="C59" s="11">
@@ -2491,17 +2488,17 @@
       <c r="E59" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="F59" s="18" t="s">
-        <v>13</v>
-      </c>
-      <c r="G59" s="19"/>
+      <c r="F59" s="25" t="s">
+        <v>13</v>
+      </c>
+      <c r="G59" s="26"/>
       <c r="H59" s="3" t="s">
         <v>182</v>
       </c>
     </row>
     <row r="60" spans="1:8" ht="171.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A60" s="21"/>
-      <c r="B60" s="24"/>
+      <c r="A60" s="39"/>
+      <c r="B60" s="42"/>
       <c r="C60" s="11">
         <v>122</v>
       </c>
@@ -2511,17 +2508,17 @@
       <c r="E60" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="F60" s="18" t="s">
-        <v>13</v>
-      </c>
-      <c r="G60" s="19"/>
+      <c r="F60" s="25" t="s">
+        <v>13</v>
+      </c>
+      <c r="G60" s="26"/>
       <c r="H60" s="3" t="s">
         <v>182</v>
       </c>
     </row>
     <row r="61" spans="1:8" ht="171.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A61" s="22"/>
-      <c r="B61" s="25"/>
+      <c r="A61" s="28"/>
+      <c r="B61" s="35"/>
       <c r="C61" s="11">
         <v>123</v>
       </c>
@@ -2531,17 +2528,17 @@
       <c r="E61" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="F61" s="18" t="s">
-        <v>13</v>
-      </c>
-      <c r="G61" s="19"/>
+      <c r="F61" s="25" t="s">
+        <v>13</v>
+      </c>
+      <c r="G61" s="26"/>
       <c r="H61" s="3" t="s">
         <v>182</v>
       </c>
     </row>
     <row r="62" spans="1:8" ht="171.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A62" s="26"/>
-      <c r="B62" s="26"/>
+      <c r="A62" s="36"/>
+      <c r="B62" s="36"/>
       <c r="C62" s="11">
         <v>124</v>
       </c>
@@ -2551,17 +2548,17 @@
       <c r="E62" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="F62" s="18" t="s">
-        <v>13</v>
-      </c>
-      <c r="G62" s="19"/>
+      <c r="F62" s="25" t="s">
+        <v>13</v>
+      </c>
+      <c r="G62" s="26"/>
       <c r="H62" s="3" t="s">
         <v>182</v>
       </c>
     </row>
     <row r="63" spans="1:8" ht="171.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A63" s="27"/>
-      <c r="B63" s="27"/>
+      <c r="A63" s="37"/>
+      <c r="B63" s="37"/>
       <c r="C63" s="11">
         <v>125</v>
       </c>
@@ -2571,17 +2568,17 @@
       <c r="E63" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="F63" s="18" t="s">
-        <v>13</v>
-      </c>
-      <c r="G63" s="19"/>
+      <c r="F63" s="25" t="s">
+        <v>13</v>
+      </c>
+      <c r="G63" s="26"/>
       <c r="H63" s="3" t="s">
         <v>182</v>
       </c>
     </row>
     <row r="64" spans="1:8" ht="171.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A64" s="28"/>
-      <c r="B64" s="28"/>
+      <c r="A64" s="38"/>
+      <c r="B64" s="38"/>
       <c r="C64" s="11">
         <v>126</v>
       </c>
@@ -2591,19 +2588,19 @@
       <c r="E64" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="F64" s="18" t="s">
-        <v>13</v>
-      </c>
-      <c r="G64" s="19"/>
+      <c r="F64" s="25" t="s">
+        <v>13</v>
+      </c>
+      <c r="G64" s="26"/>
       <c r="H64" s="3" t="s">
         <v>182</v>
       </c>
     </row>
     <row r="65" spans="1:8" ht="171.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A65" s="20">
-        <v>13</v>
-      </c>
-      <c r="B65" s="23" t="s">
+      <c r="A65" s="27">
+        <v>13</v>
+      </c>
+      <c r="B65" s="34" t="s">
         <v>100</v>
       </c>
       <c r="C65" s="11">
@@ -2615,17 +2612,17 @@
       <c r="E65" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="F65" s="18" t="s">
-        <v>13</v>
-      </c>
-      <c r="G65" s="19"/>
+      <c r="F65" s="25" t="s">
+        <v>13</v>
+      </c>
+      <c r="G65" s="26"/>
       <c r="H65" s="3" t="s">
         <v>182</v>
       </c>
     </row>
     <row r="66" spans="1:8" ht="171.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A66" s="21"/>
-      <c r="B66" s="24"/>
+      <c r="A66" s="39"/>
+      <c r="B66" s="42"/>
       <c r="C66" s="11">
         <v>132</v>
       </c>
@@ -2635,17 +2632,17 @@
       <c r="E66" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="F66" s="18" t="s">
-        <v>13</v>
-      </c>
-      <c r="G66" s="19"/>
+      <c r="F66" s="25" t="s">
+        <v>13</v>
+      </c>
+      <c r="G66" s="26"/>
       <c r="H66" s="3" t="s">
         <v>182</v>
       </c>
     </row>
     <row r="67" spans="1:8" ht="171.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A67" s="21"/>
-      <c r="B67" s="24"/>
+      <c r="A67" s="39"/>
+      <c r="B67" s="42"/>
       <c r="C67" s="11">
         <v>133</v>
       </c>
@@ -2655,17 +2652,17 @@
       <c r="E67" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="F67" s="18" t="s">
-        <v>13</v>
-      </c>
-      <c r="G67" s="19"/>
+      <c r="F67" s="25" t="s">
+        <v>13</v>
+      </c>
+      <c r="G67" s="26"/>
       <c r="H67" s="3" t="s">
         <v>182</v>
       </c>
     </row>
     <row r="68" spans="1:8" ht="171.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A68" s="21"/>
-      <c r="B68" s="24"/>
+      <c r="A68" s="39"/>
+      <c r="B68" s="42"/>
       <c r="C68" s="11">
         <v>134</v>
       </c>
@@ -2675,17 +2672,17 @@
       <c r="E68" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="F68" s="18" t="s">
-        <v>13</v>
-      </c>
-      <c r="G68" s="19"/>
+      <c r="F68" s="25" t="s">
+        <v>13</v>
+      </c>
+      <c r="G68" s="26"/>
       <c r="H68" s="3" t="s">
         <v>182</v>
       </c>
     </row>
     <row r="69" spans="1:8" ht="171.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A69" s="21"/>
-      <c r="B69" s="24"/>
+      <c r="A69" s="39"/>
+      <c r="B69" s="42"/>
       <c r="C69" s="11">
         <v>135</v>
       </c>
@@ -2695,17 +2692,17 @@
       <c r="E69" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="F69" s="18" t="s">
-        <v>13</v>
-      </c>
-      <c r="G69" s="19"/>
+      <c r="F69" s="25" t="s">
+        <v>13</v>
+      </c>
+      <c r="G69" s="26"/>
       <c r="H69" s="3" t="s">
         <v>182</v>
       </c>
     </row>
     <row r="70" spans="1:8" ht="171.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A70" s="22"/>
-      <c r="B70" s="25"/>
+      <c r="A70" s="28"/>
+      <c r="B70" s="35"/>
       <c r="C70" s="11">
         <v>136</v>
       </c>
@@ -2715,19 +2712,19 @@
       <c r="E70" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="F70" s="18" t="s">
-        <v>13</v>
-      </c>
-      <c r="G70" s="19"/>
+      <c r="F70" s="25" t="s">
+        <v>13</v>
+      </c>
+      <c r="G70" s="26"/>
       <c r="H70" s="3" t="s">
         <v>182</v>
       </c>
     </row>
     <row r="71" spans="1:8" ht="171.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A71" s="20">
+      <c r="A71" s="27">
         <v>14</v>
       </c>
-      <c r="B71" s="23" t="s">
+      <c r="B71" s="34" t="s">
         <v>107</v>
       </c>
       <c r="C71" s="11">
@@ -2739,17 +2736,17 @@
       <c r="E71" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="F71" s="18" t="s">
-        <v>13</v>
-      </c>
-      <c r="G71" s="19"/>
+      <c r="F71" s="25" t="s">
+        <v>13</v>
+      </c>
+      <c r="G71" s="26"/>
       <c r="H71" s="3" t="s">
         <v>182</v>
       </c>
     </row>
     <row r="72" spans="1:8" ht="171.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A72" s="21"/>
-      <c r="B72" s="24"/>
+      <c r="A72" s="39"/>
+      <c r="B72" s="42"/>
       <c r="C72" s="11">
         <v>142</v>
       </c>
@@ -2759,17 +2756,17 @@
       <c r="E72" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="F72" s="18" t="s">
-        <v>13</v>
-      </c>
-      <c r="G72" s="19"/>
+      <c r="F72" s="25" t="s">
+        <v>13</v>
+      </c>
+      <c r="G72" s="26"/>
       <c r="H72" s="3" t="s">
         <v>182</v>
       </c>
     </row>
     <row r="73" spans="1:8" ht="43.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A73" s="21"/>
-      <c r="B73" s="24"/>
+      <c r="A73" s="39"/>
+      <c r="B73" s="42"/>
       <c r="C73" s="11">
         <v>143</v>
       </c>
@@ -2779,17 +2776,17 @@
       <c r="E73" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="F73" s="18" t="s">
-        <v>13</v>
-      </c>
-      <c r="G73" s="19"/>
+      <c r="F73" s="25" t="s">
+        <v>13</v>
+      </c>
+      <c r="G73" s="26"/>
       <c r="H73" s="3" t="s">
         <v>110</v>
       </c>
     </row>
     <row r="74" spans="1:8" ht="43.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A74" s="21"/>
-      <c r="B74" s="24"/>
+      <c r="A74" s="39"/>
+      <c r="B74" s="42"/>
       <c r="C74" s="11">
         <v>144</v>
       </c>
@@ -2799,17 +2796,17 @@
       <c r="E74" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="F74" s="18" t="s">
-        <v>13</v>
-      </c>
-      <c r="G74" s="19"/>
+      <c r="F74" s="25" t="s">
+        <v>13</v>
+      </c>
+      <c r="G74" s="26"/>
       <c r="H74" s="3" t="s">
         <v>110</v>
       </c>
     </row>
     <row r="75" spans="1:8" ht="43.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A75" s="22"/>
-      <c r="B75" s="25"/>
+      <c r="A75" s="28"/>
+      <c r="B75" s="35"/>
       <c r="C75" s="11">
         <v>145</v>
       </c>
@@ -2819,19 +2816,19 @@
       <c r="E75" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="F75" s="18" t="s">
-        <v>13</v>
-      </c>
-      <c r="G75" s="19"/>
+      <c r="F75" s="25" t="s">
+        <v>13</v>
+      </c>
+      <c r="G75" s="26"/>
       <c r="H75" s="3" t="s">
         <v>110</v>
       </c>
     </row>
     <row r="76" spans="1:8" ht="171.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A76" s="20">
+      <c r="A76" s="27">
         <v>15</v>
       </c>
-      <c r="B76" s="23" t="s">
+      <c r="B76" s="34" t="s">
         <v>113</v>
       </c>
       <c r="C76" s="11">
@@ -2843,17 +2840,17 @@
       <c r="E76" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="F76" s="18" t="s">
-        <v>13</v>
-      </c>
-      <c r="G76" s="19"/>
+      <c r="F76" s="25" t="s">
+        <v>13</v>
+      </c>
+      <c r="G76" s="26"/>
       <c r="H76" s="3" t="s">
         <v>182</v>
       </c>
     </row>
     <row r="77" spans="1:8" ht="171.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A77" s="21"/>
-      <c r="B77" s="24"/>
+      <c r="A77" s="39"/>
+      <c r="B77" s="42"/>
       <c r="C77" s="11">
         <v>152</v>
       </c>
@@ -2863,17 +2860,17 @@
       <c r="E77" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="F77" s="18" t="s">
-        <v>13</v>
-      </c>
-      <c r="G77" s="19"/>
+      <c r="F77" s="25" t="s">
+        <v>13</v>
+      </c>
+      <c r="G77" s="26"/>
       <c r="H77" s="3" t="s">
         <v>182</v>
       </c>
     </row>
     <row r="78" spans="1:8" ht="171.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A78" s="22"/>
-      <c r="B78" s="25"/>
+      <c r="A78" s="28"/>
+      <c r="B78" s="35"/>
       <c r="C78" s="11">
         <v>153</v>
       </c>
@@ -2883,19 +2880,19 @@
       <c r="E78" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="F78" s="18" t="s">
-        <v>13</v>
-      </c>
-      <c r="G78" s="19"/>
+      <c r="F78" s="25" t="s">
+        <v>13</v>
+      </c>
+      <c r="G78" s="26"/>
       <c r="H78" s="3" t="s">
         <v>182</v>
       </c>
     </row>
     <row r="79" spans="1:8" ht="171.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A79" s="20">
+      <c r="A79" s="27">
         <v>16</v>
       </c>
-      <c r="B79" s="23" t="s">
+      <c r="B79" s="34" t="s">
         <v>117</v>
       </c>
       <c r="C79" s="11">
@@ -2907,17 +2904,17 @@
       <c r="E79" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="F79" s="18" t="s">
-        <v>13</v>
-      </c>
-      <c r="G79" s="19"/>
+      <c r="F79" s="25" t="s">
+        <v>13</v>
+      </c>
+      <c r="G79" s="26"/>
       <c r="H79" s="3" t="s">
         <v>182</v>
       </c>
     </row>
     <row r="80" spans="1:8" ht="186" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A80" s="21"/>
-      <c r="B80" s="24"/>
+      <c r="A80" s="39"/>
+      <c r="B80" s="42"/>
       <c r="C80" s="11">
         <v>162</v>
       </c>
@@ -2927,17 +2924,17 @@
       <c r="E80" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="F80" s="18" t="s">
+      <c r="F80" s="25" t="s">
         <v>27</v>
       </c>
-      <c r="G80" s="19"/>
+      <c r="G80" s="26"/>
       <c r="H80" s="3" t="s">
         <v>184</v>
       </c>
     </row>
     <row r="81" spans="1:8" ht="186" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A81" s="22"/>
-      <c r="B81" s="25"/>
+      <c r="A81" s="28"/>
+      <c r="B81" s="35"/>
       <c r="C81" s="11">
         <v>163</v>
       </c>
@@ -2947,19 +2944,19 @@
       <c r="E81" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="F81" s="18" t="s">
+      <c r="F81" s="25" t="s">
         <v>27</v>
       </c>
-      <c r="G81" s="19"/>
+      <c r="G81" s="26"/>
       <c r="H81" s="3" t="s">
         <v>184</v>
       </c>
     </row>
     <row r="82" spans="1:8" ht="171.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A82" s="20">
+      <c r="A82" s="27">
         <v>17</v>
       </c>
-      <c r="B82" s="23" t="s">
+      <c r="B82" s="34" t="s">
         <v>121</v>
       </c>
       <c r="C82" s="11">
@@ -2971,17 +2968,17 @@
       <c r="E82" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="F82" s="18" t="s">
-        <v>13</v>
-      </c>
-      <c r="G82" s="19"/>
+      <c r="F82" s="25" t="s">
+        <v>13</v>
+      </c>
+      <c r="G82" s="26"/>
       <c r="H82" s="3" t="s">
         <v>182</v>
       </c>
     </row>
     <row r="83" spans="1:8" ht="171.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A83" s="21"/>
-      <c r="B83" s="24"/>
+      <c r="A83" s="39"/>
+      <c r="B83" s="42"/>
       <c r="C83" s="11">
         <v>172</v>
       </c>
@@ -2991,17 +2988,17 @@
       <c r="E83" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="F83" s="18" t="s">
-        <v>13</v>
-      </c>
-      <c r="G83" s="19"/>
+      <c r="F83" s="25" t="s">
+        <v>13</v>
+      </c>
+      <c r="G83" s="26"/>
       <c r="H83" s="3" t="s">
         <v>182</v>
       </c>
     </row>
     <row r="84" spans="1:8" ht="171.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A84" s="22"/>
-      <c r="B84" s="25"/>
+      <c r="A84" s="28"/>
+      <c r="B84" s="35"/>
       <c r="C84" s="11">
         <v>173</v>
       </c>
@@ -3011,19 +3008,19 @@
       <c r="E84" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="F84" s="18" t="s">
-        <v>13</v>
-      </c>
-      <c r="G84" s="19"/>
+      <c r="F84" s="25" t="s">
+        <v>13</v>
+      </c>
+      <c r="G84" s="26"/>
       <c r="H84" s="3" t="s">
         <v>182</v>
       </c>
     </row>
     <row r="85" spans="1:8" ht="171.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A85" s="20">
+      <c r="A85" s="27">
         <v>18</v>
       </c>
-      <c r="B85" s="23" t="s">
+      <c r="B85" s="34" t="s">
         <v>125</v>
       </c>
       <c r="C85" s="11">
@@ -3035,17 +3032,17 @@
       <c r="E85" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="F85" s="18" t="s">
-        <v>13</v>
-      </c>
-      <c r="G85" s="19"/>
+      <c r="F85" s="25" t="s">
+        <v>13</v>
+      </c>
+      <c r="G85" s="26"/>
       <c r="H85" s="3" t="s">
         <v>182</v>
       </c>
     </row>
     <row r="86" spans="1:8" ht="171.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A86" s="21"/>
-      <c r="B86" s="24"/>
+      <c r="A86" s="39"/>
+      <c r="B86" s="42"/>
       <c r="C86" s="11">
         <v>182</v>
       </c>
@@ -3055,17 +3052,17 @@
       <c r="E86" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="F86" s="18" t="s">
-        <v>13</v>
-      </c>
-      <c r="G86" s="19"/>
+      <c r="F86" s="25" t="s">
+        <v>13</v>
+      </c>
+      <c r="G86" s="26"/>
       <c r="H86" s="3" t="s">
         <v>182</v>
       </c>
     </row>
     <row r="87" spans="1:8" ht="171.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A87" s="21"/>
-      <c r="B87" s="24"/>
+      <c r="A87" s="39"/>
+      <c r="B87" s="42"/>
       <c r="C87" s="11">
         <v>183</v>
       </c>
@@ -3075,17 +3072,17 @@
       <c r="E87" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="F87" s="18" t="s">
-        <v>13</v>
-      </c>
-      <c r="G87" s="19"/>
+      <c r="F87" s="25" t="s">
+        <v>13</v>
+      </c>
+      <c r="G87" s="26"/>
       <c r="H87" s="3" t="s">
         <v>182</v>
       </c>
     </row>
     <row r="88" spans="1:8" ht="171.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A88" s="21"/>
-      <c r="B88" s="24"/>
+      <c r="A88" s="39"/>
+      <c r="B88" s="42"/>
       <c r="C88" s="11">
         <v>184</v>
       </c>
@@ -3095,17 +3092,17 @@
       <c r="E88" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="F88" s="18" t="s">
-        <v>13</v>
-      </c>
-      <c r="G88" s="19"/>
+      <c r="F88" s="25" t="s">
+        <v>13</v>
+      </c>
+      <c r="G88" s="26"/>
       <c r="H88" s="3" t="s">
         <v>182</v>
       </c>
     </row>
     <row r="89" spans="1:8" ht="171.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A89" s="21"/>
-      <c r="B89" s="24"/>
+      <c r="A89" s="39"/>
+      <c r="B89" s="42"/>
       <c r="C89" s="11">
         <v>185</v>
       </c>
@@ -3115,17 +3112,17 @@
       <c r="E89" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="F89" s="18" t="s">
-        <v>13</v>
-      </c>
-      <c r="G89" s="19"/>
+      <c r="F89" s="25" t="s">
+        <v>13</v>
+      </c>
+      <c r="G89" s="26"/>
       <c r="H89" s="3" t="s">
         <v>182</v>
       </c>
     </row>
     <row r="90" spans="1:8" ht="171.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A90" s="22"/>
-      <c r="B90" s="25"/>
+      <c r="A90" s="28"/>
+      <c r="B90" s="35"/>
       <c r="C90" s="11">
         <v>186</v>
       </c>
@@ -3135,10 +3132,10 @@
       <c r="E90" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="F90" s="18" t="s">
-        <v>13</v>
-      </c>
-      <c r="G90" s="19"/>
+      <c r="F90" s="25" t="s">
+        <v>13</v>
+      </c>
+      <c r="G90" s="26"/>
       <c r="H90" s="3" t="s">
         <v>182</v>
       </c>
@@ -3155,19 +3152,19 @@
       <c r="E91" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="F91" s="18" t="s">
-        <v>13</v>
-      </c>
-      <c r="G91" s="19"/>
+      <c r="F91" s="25" t="s">
+        <v>13</v>
+      </c>
+      <c r="G91" s="26"/>
       <c r="H91" s="3" t="s">
         <v>182</v>
       </c>
     </row>
     <row r="92" spans="1:8" ht="72" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A92" s="20">
+      <c r="A92" s="27">
         <v>19</v>
       </c>
-      <c r="B92" s="23" t="s">
+      <c r="B92" s="34" t="s">
         <v>133</v>
       </c>
       <c r="C92" s="11">
@@ -3179,17 +3176,17 @@
       <c r="E92" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="F92" s="18" t="s">
-        <v>13</v>
-      </c>
-      <c r="G92" s="19"/>
+      <c r="F92" s="25" t="s">
+        <v>13</v>
+      </c>
+      <c r="G92" s="26"/>
       <c r="H92" s="3" t="s">
         <v>51</v>
       </c>
     </row>
     <row r="93" spans="1:8" ht="171.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A93" s="21"/>
-      <c r="B93" s="24"/>
+      <c r="A93" s="39"/>
+      <c r="B93" s="42"/>
       <c r="C93" s="11">
         <v>192</v>
       </c>
@@ -3199,17 +3196,17 @@
       <c r="E93" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="F93" s="18" t="s">
-        <v>13</v>
-      </c>
-      <c r="G93" s="19"/>
+      <c r="F93" s="25" t="s">
+        <v>13</v>
+      </c>
+      <c r="G93" s="26"/>
       <c r="H93" s="3" t="s">
         <v>182</v>
       </c>
     </row>
     <row r="94" spans="1:8" ht="171.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A94" s="21"/>
-      <c r="B94" s="24"/>
+      <c r="A94" s="39"/>
+      <c r="B94" s="42"/>
       <c r="C94" s="11">
         <v>193</v>
       </c>
@@ -3219,17 +3216,17 @@
       <c r="E94" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="F94" s="18" t="s">
-        <v>13</v>
-      </c>
-      <c r="G94" s="19"/>
+      <c r="F94" s="25" t="s">
+        <v>13</v>
+      </c>
+      <c r="G94" s="26"/>
       <c r="H94" s="3" t="s">
         <v>182</v>
       </c>
     </row>
     <row r="95" spans="1:8" ht="171.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A95" s="22"/>
-      <c r="B95" s="25"/>
+      <c r="A95" s="28"/>
+      <c r="B95" s="35"/>
       <c r="C95" s="11">
         <v>194</v>
       </c>
@@ -3239,19 +3236,19 @@
       <c r="E95" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="F95" s="18" t="s">
-        <v>13</v>
-      </c>
-      <c r="G95" s="19"/>
+      <c r="F95" s="25" t="s">
+        <v>13</v>
+      </c>
+      <c r="G95" s="26"/>
       <c r="H95" s="3" t="s">
         <v>182</v>
       </c>
     </row>
     <row r="96" spans="1:8" ht="186" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A96" s="20">
+      <c r="A96" s="27">
         <v>20</v>
       </c>
-      <c r="B96" s="23" t="s">
+      <c r="B96" s="34" t="s">
         <v>137</v>
       </c>
       <c r="C96" s="11">
@@ -3263,17 +3260,17 @@
       <c r="E96" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="F96" s="18" t="s">
+      <c r="F96" s="25" t="s">
         <v>27</v>
       </c>
-      <c r="G96" s="19"/>
+      <c r="G96" s="26"/>
       <c r="H96" s="3" t="s">
         <v>184</v>
       </c>
     </row>
     <row r="97" spans="1:8" ht="186" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A97" s="21"/>
-      <c r="B97" s="24"/>
+      <c r="A97" s="39"/>
+      <c r="B97" s="42"/>
       <c r="C97" s="11">
         <v>202</v>
       </c>
@@ -3283,17 +3280,17 @@
       <c r="E97" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="F97" s="18" t="s">
+      <c r="F97" s="25" t="s">
         <v>27</v>
       </c>
-      <c r="G97" s="19"/>
+      <c r="G97" s="26"/>
       <c r="H97" s="3" t="s">
         <v>184</v>
       </c>
     </row>
     <row r="98" spans="1:8" ht="186" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A98" s="21"/>
-      <c r="B98" s="24"/>
+      <c r="A98" s="39"/>
+      <c r="B98" s="42"/>
       <c r="C98" s="11">
         <v>203</v>
       </c>
@@ -3303,17 +3300,17 @@
       <c r="E98" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="F98" s="18" t="s">
+      <c r="F98" s="25" t="s">
         <v>27</v>
       </c>
-      <c r="G98" s="19"/>
+      <c r="G98" s="26"/>
       <c r="H98" s="3" t="s">
         <v>184</v>
       </c>
     </row>
     <row r="99" spans="1:8" ht="186" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A99" s="22"/>
-      <c r="B99" s="25"/>
+      <c r="A99" s="28"/>
+      <c r="B99" s="35"/>
       <c r="C99" s="11">
         <v>204</v>
       </c>
@@ -3323,17 +3320,17 @@
       <c r="E99" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="F99" s="18" t="s">
+      <c r="F99" s="25" t="s">
         <v>27</v>
       </c>
-      <c r="G99" s="19"/>
+      <c r="G99" s="26"/>
       <c r="H99" s="3" t="s">
         <v>184</v>
       </c>
     </row>
     <row r="100" spans="1:8" ht="171.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A100" s="26"/>
-      <c r="B100" s="26"/>
+      <c r="A100" s="36"/>
+      <c r="B100" s="36"/>
       <c r="C100" s="11">
         <v>205</v>
       </c>
@@ -3343,17 +3340,17 @@
       <c r="E100" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="F100" s="18" t="s">
-        <v>13</v>
-      </c>
-      <c r="G100" s="19"/>
+      <c r="F100" s="25" t="s">
+        <v>13</v>
+      </c>
+      <c r="G100" s="26"/>
       <c r="H100" s="3" t="s">
         <v>182</v>
       </c>
     </row>
     <row r="101" spans="1:8" ht="171.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A101" s="27"/>
-      <c r="B101" s="27"/>
+      <c r="A101" s="37"/>
+      <c r="B101" s="37"/>
       <c r="C101" s="11">
         <v>206</v>
       </c>
@@ -3363,17 +3360,17 @@
       <c r="E101" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="F101" s="18" t="s">
-        <v>13</v>
-      </c>
-      <c r="G101" s="19"/>
+      <c r="F101" s="25" t="s">
+        <v>13</v>
+      </c>
+      <c r="G101" s="26"/>
       <c r="H101" s="3" t="s">
         <v>182</v>
       </c>
     </row>
     <row r="102" spans="1:8" ht="186" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A102" s="27"/>
-      <c r="B102" s="27"/>
+      <c r="A102" s="37"/>
+      <c r="B102" s="37"/>
       <c r="C102" s="11">
         <v>207</v>
       </c>
@@ -3383,17 +3380,17 @@
       <c r="E102" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="F102" s="18" t="s">
+      <c r="F102" s="25" t="s">
         <v>27</v>
       </c>
-      <c r="G102" s="19"/>
+      <c r="G102" s="26"/>
       <c r="H102" s="3" t="s">
         <v>184</v>
       </c>
     </row>
     <row r="103" spans="1:8" ht="171.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A103" s="28"/>
-      <c r="B103" s="28"/>
+      <c r="A103" s="38"/>
+      <c r="B103" s="38"/>
       <c r="C103" s="11">
         <v>208</v>
       </c>
@@ -3403,19 +3400,19 @@
       <c r="E103" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="F103" s="18" t="s">
-        <v>13</v>
-      </c>
-      <c r="G103" s="19"/>
+      <c r="F103" s="25" t="s">
+        <v>13</v>
+      </c>
+      <c r="G103" s="26"/>
       <c r="H103" s="3" t="s">
         <v>182</v>
       </c>
     </row>
     <row r="104" spans="1:8" ht="57.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A104" s="20">
+      <c r="A104" s="27">
         <v>21</v>
       </c>
-      <c r="B104" s="23" t="s">
+      <c r="B104" s="34" t="s">
         <v>146</v>
       </c>
       <c r="C104" s="11">
@@ -3427,17 +3424,17 @@
       <c r="E104" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="F104" s="18" t="s">
+      <c r="F104" s="25" t="s">
         <v>147</v>
       </c>
-      <c r="G104" s="19"/>
+      <c r="G104" s="26"/>
       <c r="H104" s="3" t="s">
         <v>148</v>
       </c>
     </row>
     <row r="105" spans="1:8" ht="100.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A105" s="22"/>
-      <c r="B105" s="25"/>
+      <c r="A105" s="28"/>
+      <c r="B105" s="35"/>
       <c r="C105" s="11">
         <v>212</v>
       </c>
@@ -3447,19 +3444,19 @@
       <c r="E105" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="F105" s="18" t="s">
+      <c r="F105" s="25" t="s">
         <v>147</v>
       </c>
-      <c r="G105" s="19"/>
+      <c r="G105" s="26"/>
       <c r="H105" s="3" t="s">
         <v>148</v>
       </c>
     </row>
     <row r="106" spans="1:8" ht="72" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A106" s="20">
+      <c r="A106" s="27">
         <v>22</v>
       </c>
-      <c r="B106" s="23" t="s">
+      <c r="B106" s="34" t="s">
         <v>149</v>
       </c>
       <c r="C106" s="11">
@@ -3471,17 +3468,17 @@
       <c r="E106" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="F106" s="18" t="s">
-        <v>13</v>
-      </c>
-      <c r="G106" s="19"/>
+      <c r="F106" s="25" t="s">
+        <v>13</v>
+      </c>
+      <c r="G106" s="26"/>
       <c r="H106" s="3" t="s">
         <v>199</v>
       </c>
     </row>
     <row r="107" spans="1:8" ht="72" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A107" s="21"/>
-      <c r="B107" s="24"/>
+      <c r="A107" s="39"/>
+      <c r="B107" s="42"/>
       <c r="C107" s="11">
         <v>222</v>
       </c>
@@ -3491,17 +3488,17 @@
       <c r="E107" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="F107" s="18" t="s">
-        <v>13</v>
-      </c>
-      <c r="G107" s="19"/>
+      <c r="F107" s="25" t="s">
+        <v>13</v>
+      </c>
+      <c r="G107" s="26"/>
       <c r="H107" s="3" t="s">
         <v>199</v>
       </c>
     </row>
     <row r="108" spans="1:8" ht="72" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A108" s="21"/>
-      <c r="B108" s="24"/>
+      <c r="A108" s="39"/>
+      <c r="B108" s="42"/>
       <c r="C108" s="11">
         <v>223</v>
       </c>
@@ -3511,17 +3508,17 @@
       <c r="E108" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="F108" s="18" t="s">
-        <v>13</v>
-      </c>
-      <c r="G108" s="19"/>
+      <c r="F108" s="25" t="s">
+        <v>13</v>
+      </c>
+      <c r="G108" s="26"/>
       <c r="H108" s="3" t="s">
         <v>199</v>
       </c>
     </row>
     <row r="109" spans="1:8" ht="114.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A109" s="21"/>
-      <c r="B109" s="24"/>
+      <c r="A109" s="39"/>
+      <c r="B109" s="42"/>
       <c r="C109" s="11">
         <v>224</v>
       </c>
@@ -3531,17 +3528,17 @@
       <c r="E109" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="F109" s="18" t="s">
-        <v>13</v>
-      </c>
-      <c r="G109" s="19"/>
+      <c r="F109" s="25" t="s">
+        <v>13</v>
+      </c>
+      <c r="G109" s="26"/>
       <c r="H109" s="3" t="s">
         <v>199</v>
       </c>
     </row>
     <row r="110" spans="1:8" ht="72" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A110" s="21"/>
-      <c r="B110" s="24"/>
+      <c r="A110" s="39"/>
+      <c r="B110" s="42"/>
       <c r="C110" s="11">
         <v>225</v>
       </c>
@@ -3551,17 +3548,17 @@
       <c r="E110" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="F110" s="18" t="s">
-        <v>13</v>
-      </c>
-      <c r="G110" s="19"/>
+      <c r="F110" s="25" t="s">
+        <v>13</v>
+      </c>
+      <c r="G110" s="26"/>
       <c r="H110" s="3" t="s">
         <v>199</v>
       </c>
     </row>
     <row r="111" spans="1:8" ht="86.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A111" s="21"/>
-      <c r="B111" s="24"/>
+      <c r="A111" s="39"/>
+      <c r="B111" s="42"/>
       <c r="C111" s="11">
         <v>226</v>
       </c>
@@ -3571,17 +3568,17 @@
       <c r="E111" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="F111" s="18" t="s">
-        <v>13</v>
-      </c>
-      <c r="G111" s="19"/>
+      <c r="F111" s="25" t="s">
+        <v>13</v>
+      </c>
+      <c r="G111" s="26"/>
       <c r="H111" s="3" t="s">
         <v>199</v>
       </c>
     </row>
     <row r="112" spans="1:8" ht="72" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A112" s="21"/>
-      <c r="B112" s="24"/>
+      <c r="A112" s="39"/>
+      <c r="B112" s="42"/>
       <c r="C112" s="11">
         <v>227</v>
       </c>
@@ -3591,17 +3588,17 @@
       <c r="E112" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="F112" s="18" t="s">
-        <v>13</v>
-      </c>
-      <c r="G112" s="19"/>
+      <c r="F112" s="25" t="s">
+        <v>13</v>
+      </c>
+      <c r="G112" s="26"/>
       <c r="H112" s="3" t="s">
         <v>199</v>
       </c>
     </row>
     <row r="113" spans="1:8" ht="72" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A113" s="21"/>
-      <c r="B113" s="24"/>
+      <c r="A113" s="39"/>
+      <c r="B113" s="42"/>
       <c r="C113" s="11">
         <v>228</v>
       </c>
@@ -3611,17 +3608,17 @@
       <c r="E113" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="F113" s="18" t="s">
-        <v>13</v>
-      </c>
-      <c r="G113" s="19"/>
+      <c r="F113" s="25" t="s">
+        <v>13</v>
+      </c>
+      <c r="G113" s="26"/>
       <c r="H113" s="3" t="s">
         <v>199</v>
       </c>
     </row>
     <row r="114" spans="1:8" ht="72" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A114" s="22"/>
-      <c r="B114" s="25"/>
+      <c r="A114" s="28"/>
+      <c r="B114" s="35"/>
       <c r="C114" s="11">
         <v>229</v>
       </c>
@@ -3631,19 +3628,19 @@
       <c r="E114" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="F114" s="18" t="s">
-        <v>13</v>
-      </c>
-      <c r="G114" s="19"/>
+      <c r="F114" s="25" t="s">
+        <v>13</v>
+      </c>
+      <c r="G114" s="26"/>
       <c r="H114" s="3" t="s">
         <v>199</v>
       </c>
     </row>
     <row r="115" spans="1:8" ht="171.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A115" s="20">
+      <c r="A115" s="27">
         <v>23</v>
       </c>
-      <c r="B115" s="23" t="s">
+      <c r="B115" s="34" t="s">
         <v>157</v>
       </c>
       <c r="C115" s="11">
@@ -3655,17 +3652,17 @@
       <c r="E115" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="F115" s="18" t="s">
-        <v>13</v>
-      </c>
-      <c r="G115" s="19"/>
+      <c r="F115" s="25" t="s">
+        <v>13</v>
+      </c>
+      <c r="G115" s="26"/>
       <c r="H115" s="3" t="s">
         <v>193</v>
       </c>
     </row>
     <row r="116" spans="1:8" ht="171.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A116" s="22"/>
-      <c r="B116" s="25"/>
+      <c r="A116" s="28"/>
+      <c r="B116" s="35"/>
       <c r="C116" s="11">
         <v>232</v>
       </c>
@@ -3675,19 +3672,19 @@
       <c r="E116" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="F116" s="18" t="s">
-        <v>13</v>
-      </c>
-      <c r="G116" s="19"/>
+      <c r="F116" s="25" t="s">
+        <v>13</v>
+      </c>
+      <c r="G116" s="26"/>
       <c r="H116" s="3" t="s">
         <v>193</v>
       </c>
     </row>
     <row r="117" spans="1:8" ht="171.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A117" s="20">
-        <v>24</v>
-      </c>
-      <c r="B117" s="23" t="s">
+      <c r="A117" s="27">
+        <v>24</v>
+      </c>
+      <c r="B117" s="34" t="s">
         <v>159</v>
       </c>
       <c r="C117" s="11">
@@ -3699,17 +3696,17 @@
       <c r="E117" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="F117" s="18" t="s">
+      <c r="F117" s="25" t="s">
         <v>19</v>
       </c>
-      <c r="G117" s="19"/>
+      <c r="G117" s="26"/>
       <c r="H117" s="3" t="s">
         <v>183</v>
       </c>
     </row>
     <row r="118" spans="1:8" ht="171.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A118" s="22"/>
-      <c r="B118" s="25"/>
+      <c r="A118" s="28"/>
+      <c r="B118" s="35"/>
       <c r="C118" s="11">
         <v>242</v>
       </c>
@@ -3719,63 +3716,63 @@
       <c r="E118" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="F118" s="18" t="s">
+      <c r="F118" s="25" t="s">
         <v>19</v>
       </c>
-      <c r="G118" s="19"/>
+      <c r="G118" s="26"/>
       <c r="H118" s="3" t="s">
         <v>183</v>
       </c>
     </row>
     <row r="119" spans="1:8" ht="129" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A119" s="40">
+      <c r="A119" s="21">
         <v>25</v>
       </c>
-      <c r="B119" s="41" t="s">
+      <c r="B119" s="22" t="s">
         <v>202</v>
       </c>
-      <c r="C119" s="34">
+      <c r="C119" s="15">
         <v>255</v>
       </c>
-      <c r="D119" s="35" t="s">
+      <c r="D119" s="16" t="s">
         <v>203</v>
       </c>
-      <c r="E119" s="35" t="s">
-        <v>24</v>
-      </c>
-      <c r="F119" s="36" t="s">
-        <v>13</v>
-      </c>
-      <c r="G119" s="36"/>
-      <c r="H119" s="36" t="s">
+      <c r="E119" s="16" t="s">
+        <v>24</v>
+      </c>
+      <c r="F119" s="17" t="s">
+        <v>13</v>
+      </c>
+      <c r="G119" s="17"/>
+      <c r="H119" s="17" t="s">
         <v>162</v>
       </c>
     </row>
     <row r="120" spans="1:8" ht="409.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A120" s="42"/>
-      <c r="B120" s="43"/>
-      <c r="C120" s="37">
+      <c r="A120" s="23"/>
+      <c r="B120" s="24"/>
+      <c r="C120" s="18">
         <v>256</v>
       </c>
-      <c r="D120" s="37" t="s">
+      <c r="D120" s="18" t="s">
         <v>204</v>
       </c>
-      <c r="E120" s="37" t="s">
-        <v>24</v>
-      </c>
-      <c r="F120" s="38" t="s">
-        <v>13</v>
-      </c>
-      <c r="G120" s="36" t="s">
+      <c r="E120" s="18" t="s">
+        <v>24</v>
+      </c>
+      <c r="F120" s="19" t="s">
+        <v>13</v>
+      </c>
+      <c r="G120" s="17" t="s">
         <v>163</v>
       </c>
-      <c r="H120" s="39"/>
+      <c r="H120" s="20"/>
     </row>
     <row r="121" spans="1:8" ht="43.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A121" s="20">
+      <c r="A121" s="27">
         <v>26</v>
       </c>
-      <c r="B121" s="23" t="s">
+      <c r="B121" s="34" t="s">
         <v>164</v>
       </c>
       <c r="C121" s="11">
@@ -3787,17 +3784,17 @@
       <c r="E121" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="F121" s="18" t="s">
-        <v>13</v>
-      </c>
-      <c r="G121" s="19"/>
+      <c r="F121" s="25" t="s">
+        <v>13</v>
+      </c>
+      <c r="G121" s="26"/>
       <c r="H121" s="3" t="s">
         <v>166</v>
       </c>
     </row>
     <row r="122" spans="1:8" ht="409.6" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A122" s="21"/>
-      <c r="B122" s="24"/>
+      <c r="A122" s="39"/>
+      <c r="B122" s="42"/>
       <c r="C122" s="11">
         <v>261</v>
       </c>
@@ -3807,17 +3804,17 @@
       <c r="E122" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="F122" s="18" t="s">
-        <v>13</v>
-      </c>
-      <c r="G122" s="19"/>
+      <c r="F122" s="25" t="s">
+        <v>13</v>
+      </c>
+      <c r="G122" s="26"/>
       <c r="H122" s="3" t="s">
         <v>51</v>
       </c>
     </row>
     <row r="123" spans="1:8" ht="409.6" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A123" s="21"/>
-      <c r="B123" s="24"/>
+      <c r="A123" s="39"/>
+      <c r="B123" s="42"/>
       <c r="C123" s="11">
         <v>262</v>
       </c>
@@ -3827,17 +3824,17 @@
       <c r="E123" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="F123" s="18" t="s">
+      <c r="F123" s="25" t="s">
         <v>11</v>
       </c>
-      <c r="G123" s="19"/>
+      <c r="G123" s="26"/>
       <c r="H123" s="3" t="s">
         <v>51</v>
       </c>
     </row>
     <row r="124" spans="1:8" ht="409.6" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A124" s="21"/>
-      <c r="B124" s="24"/>
+      <c r="A124" s="39"/>
+      <c r="B124" s="42"/>
       <c r="C124" s="11">
         <v>262</v>
       </c>
@@ -3847,17 +3844,17 @@
       <c r="E124" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="F124" s="18" t="s">
-        <v>13</v>
-      </c>
-      <c r="G124" s="19"/>
+      <c r="F124" s="25" t="s">
+        <v>13</v>
+      </c>
+      <c r="G124" s="26"/>
       <c r="H124" s="3" t="s">
         <v>163</v>
       </c>
     </row>
     <row r="125" spans="1:8" ht="57.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A125" s="22"/>
-      <c r="B125" s="25"/>
+      <c r="A125" s="28"/>
+      <c r="B125" s="35"/>
       <c r="C125" s="11">
         <v>263</v>
       </c>
@@ -3867,19 +3864,19 @@
       <c r="E125" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="F125" s="18" t="s">
-        <v>13</v>
-      </c>
-      <c r="G125" s="19"/>
+      <c r="F125" s="25" t="s">
+        <v>13</v>
+      </c>
+      <c r="G125" s="26"/>
       <c r="H125" s="3" t="s">
         <v>162</v>
       </c>
     </row>
     <row r="126" spans="1:8" ht="86.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A126" s="20">
+      <c r="A126" s="27">
         <v>27</v>
       </c>
-      <c r="B126" s="23" t="s">
+      <c r="B126" s="34" t="s">
         <v>167</v>
       </c>
       <c r="C126" s="11">
@@ -3891,17 +3888,17 @@
       <c r="E126" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="F126" s="18" t="s">
-        <v>13</v>
-      </c>
-      <c r="G126" s="19"/>
+      <c r="F126" s="25" t="s">
+        <v>13</v>
+      </c>
+      <c r="G126" s="26"/>
       <c r="H126" s="3" t="s">
         <v>162</v>
       </c>
     </row>
     <row r="127" spans="1:8" ht="57.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A127" s="21"/>
-      <c r="B127" s="24"/>
+      <c r="A127" s="39"/>
+      <c r="B127" s="42"/>
       <c r="C127" s="11">
         <v>272</v>
       </c>
@@ -3911,17 +3908,17 @@
       <c r="E127" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="F127" s="18" t="s">
-        <v>13</v>
-      </c>
-      <c r="G127" s="19"/>
+      <c r="F127" s="25" t="s">
+        <v>13</v>
+      </c>
+      <c r="G127" s="26"/>
       <c r="H127" s="3" t="s">
         <v>162</v>
       </c>
     </row>
     <row r="128" spans="1:8" ht="57.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A128" s="21"/>
-      <c r="B128" s="24"/>
+      <c r="A128" s="39"/>
+      <c r="B128" s="42"/>
       <c r="C128" s="11">
         <v>273</v>
       </c>
@@ -3931,17 +3928,17 @@
       <c r="E128" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="F128" s="18" t="s">
-        <v>13</v>
-      </c>
-      <c r="G128" s="19"/>
+      <c r="F128" s="25" t="s">
+        <v>13</v>
+      </c>
+      <c r="G128" s="26"/>
       <c r="H128" s="3" t="s">
         <v>162</v>
       </c>
     </row>
     <row r="129" spans="1:8" ht="57.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A129" s="21"/>
-      <c r="B129" s="24"/>
+      <c r="A129" s="39"/>
+      <c r="B129" s="42"/>
       <c r="C129" s="11">
         <v>274</v>
       </c>
@@ -3951,17 +3948,17 @@
       <c r="E129" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="F129" s="18" t="s">
-        <v>13</v>
-      </c>
-      <c r="G129" s="19"/>
+      <c r="F129" s="25" t="s">
+        <v>13</v>
+      </c>
+      <c r="G129" s="26"/>
       <c r="H129" s="3" t="s">
         <v>162</v>
       </c>
     </row>
     <row r="130" spans="1:8" ht="72" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A130" s="22"/>
-      <c r="B130" s="25"/>
+      <c r="A130" s="28"/>
+      <c r="B130" s="35"/>
       <c r="C130" s="11">
         <v>275</v>
       </c>
@@ -3971,10 +3968,10 @@
       <c r="E130" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="F130" s="18" t="s">
-        <v>13</v>
-      </c>
-      <c r="G130" s="19"/>
+      <c r="F130" s="25" t="s">
+        <v>13</v>
+      </c>
+      <c r="G130" s="26"/>
       <c r="H130" s="3" t="s">
         <v>162</v>
       </c>
@@ -3995,19 +3992,19 @@
       <c r="E131" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="F131" s="18" t="s">
-        <v>13</v>
-      </c>
-      <c r="G131" s="19"/>
+      <c r="F131" s="25" t="s">
+        <v>13</v>
+      </c>
+      <c r="G131" s="26"/>
       <c r="H131" s="3" t="s">
         <v>182</v>
       </c>
     </row>
     <row r="132" spans="1:8" ht="171.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A132" s="20">
+      <c r="A132" s="27">
         <v>29</v>
       </c>
-      <c r="B132" s="23" t="s">
+      <c r="B132" s="34" t="s">
         <v>174</v>
       </c>
       <c r="C132" s="11">
@@ -4019,17 +4016,17 @@
       <c r="E132" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="F132" s="18" t="s">
+      <c r="F132" s="25" t="s">
         <v>19</v>
       </c>
-      <c r="G132" s="19"/>
+      <c r="G132" s="26"/>
       <c r="H132" s="3" t="s">
         <v>183</v>
       </c>
     </row>
     <row r="133" spans="1:8" ht="171.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A133" s="21"/>
-      <c r="B133" s="24"/>
+      <c r="A133" s="39"/>
+      <c r="B133" s="42"/>
       <c r="C133" s="11">
         <v>292</v>
       </c>
@@ -4039,17 +4036,17 @@
       <c r="E133" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="F133" s="18" t="s">
-        <v>13</v>
-      </c>
-      <c r="G133" s="19"/>
+      <c r="F133" s="25" t="s">
+        <v>13</v>
+      </c>
+      <c r="G133" s="26"/>
       <c r="H133" s="3" t="s">
         <v>182</v>
       </c>
     </row>
     <row r="134" spans="1:8" ht="72" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A134" s="22"/>
-      <c r="B134" s="25"/>
+      <c r="A134" s="28"/>
+      <c r="B134" s="35"/>
       <c r="C134" s="11">
         <v>293</v>
       </c>
@@ -4059,35 +4056,172 @@
       <c r="E134" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="F134" s="18" t="s">
+      <c r="F134" s="25" t="s">
         <v>19</v>
       </c>
-      <c r="G134" s="19"/>
+      <c r="G134" s="26"/>
       <c r="H134" s="3" t="s">
         <v>177</v>
       </c>
     </row>
-    <row r="135" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A135" s="15"/>
-      <c r="B135" s="16"/>
-      <c r="C135" s="16"/>
-      <c r="D135" s="16"/>
-      <c r="E135" s="16"/>
-      <c r="F135" s="16"/>
-      <c r="G135" s="16"/>
-      <c r="H135" s="17"/>
-    </row>
   </sheetData>
-  <mergeCells count="190">
-    <mergeCell ref="F8:G8"/>
-    <mergeCell ref="F9:G9"/>
-    <mergeCell ref="F10:G10"/>
-    <mergeCell ref="A1:A2"/>
-    <mergeCell ref="B1:B2"/>
-    <mergeCell ref="C1:C2"/>
-    <mergeCell ref="D1:D2"/>
-    <mergeCell ref="E1:H1"/>
-    <mergeCell ref="F2:G2"/>
+  <mergeCells count="189">
+    <mergeCell ref="B121:B125"/>
+    <mergeCell ref="F121:G121"/>
+    <mergeCell ref="F122:G122"/>
+    <mergeCell ref="F123:G123"/>
+    <mergeCell ref="F131:G131"/>
+    <mergeCell ref="A132:A134"/>
+    <mergeCell ref="B132:B134"/>
+    <mergeCell ref="F132:G132"/>
+    <mergeCell ref="F133:G133"/>
+    <mergeCell ref="F134:G134"/>
+    <mergeCell ref="F124:G124"/>
+    <mergeCell ref="F125:G125"/>
+    <mergeCell ref="A126:A130"/>
+    <mergeCell ref="B126:B130"/>
+    <mergeCell ref="F126:G126"/>
+    <mergeCell ref="F127:G127"/>
+    <mergeCell ref="F128:G128"/>
+    <mergeCell ref="F129:G129"/>
+    <mergeCell ref="F130:G130"/>
+    <mergeCell ref="A121:A125"/>
+    <mergeCell ref="A117:A118"/>
+    <mergeCell ref="B117:B118"/>
+    <mergeCell ref="F117:G117"/>
+    <mergeCell ref="F118:G118"/>
+    <mergeCell ref="F110:G110"/>
+    <mergeCell ref="F111:G111"/>
+    <mergeCell ref="F112:G112"/>
+    <mergeCell ref="F113:G113"/>
+    <mergeCell ref="F114:G114"/>
+    <mergeCell ref="A115:A116"/>
+    <mergeCell ref="B115:B116"/>
+    <mergeCell ref="F115:G115"/>
+    <mergeCell ref="F116:G116"/>
+    <mergeCell ref="A104:A105"/>
+    <mergeCell ref="B104:B105"/>
+    <mergeCell ref="F104:G104"/>
+    <mergeCell ref="F105:G105"/>
+    <mergeCell ref="A106:A114"/>
+    <mergeCell ref="B106:B114"/>
+    <mergeCell ref="F106:G106"/>
+    <mergeCell ref="F107:G107"/>
+    <mergeCell ref="F108:G108"/>
+    <mergeCell ref="F109:G109"/>
+    <mergeCell ref="A92:A95"/>
+    <mergeCell ref="B92:B95"/>
+    <mergeCell ref="F92:G92"/>
+    <mergeCell ref="F93:G93"/>
+    <mergeCell ref="F94:G94"/>
+    <mergeCell ref="F95:G95"/>
+    <mergeCell ref="A100:A103"/>
+    <mergeCell ref="B100:B103"/>
+    <mergeCell ref="F100:G100"/>
+    <mergeCell ref="F101:G101"/>
+    <mergeCell ref="F102:G102"/>
+    <mergeCell ref="F103:G103"/>
+    <mergeCell ref="A96:A99"/>
+    <mergeCell ref="B96:B99"/>
+    <mergeCell ref="F96:G96"/>
+    <mergeCell ref="F97:G97"/>
+    <mergeCell ref="F98:G98"/>
+    <mergeCell ref="F99:G99"/>
+    <mergeCell ref="A85:A90"/>
+    <mergeCell ref="B85:B90"/>
+    <mergeCell ref="F85:G85"/>
+    <mergeCell ref="F86:G86"/>
+    <mergeCell ref="F87:G87"/>
+    <mergeCell ref="F88:G88"/>
+    <mergeCell ref="F89:G89"/>
+    <mergeCell ref="F90:G90"/>
+    <mergeCell ref="F91:G91"/>
+    <mergeCell ref="A79:A81"/>
+    <mergeCell ref="B79:B81"/>
+    <mergeCell ref="F79:G79"/>
+    <mergeCell ref="F80:G80"/>
+    <mergeCell ref="F81:G81"/>
+    <mergeCell ref="A82:A84"/>
+    <mergeCell ref="B82:B84"/>
+    <mergeCell ref="F82:G82"/>
+    <mergeCell ref="F83:G83"/>
+    <mergeCell ref="F84:G84"/>
+    <mergeCell ref="A71:A75"/>
+    <mergeCell ref="B71:B75"/>
+    <mergeCell ref="F71:G71"/>
+    <mergeCell ref="F72:G72"/>
+    <mergeCell ref="F73:G73"/>
+    <mergeCell ref="F74:G74"/>
+    <mergeCell ref="F75:G75"/>
+    <mergeCell ref="A76:A78"/>
+    <mergeCell ref="B76:B78"/>
+    <mergeCell ref="F76:G76"/>
+    <mergeCell ref="F77:G77"/>
+    <mergeCell ref="F78:G78"/>
+    <mergeCell ref="A62:A64"/>
+    <mergeCell ref="B62:B64"/>
+    <mergeCell ref="F62:G62"/>
+    <mergeCell ref="F63:G63"/>
+    <mergeCell ref="F64:G64"/>
+    <mergeCell ref="A65:A70"/>
+    <mergeCell ref="B65:B70"/>
+    <mergeCell ref="F65:G65"/>
+    <mergeCell ref="F66:G66"/>
+    <mergeCell ref="F67:G67"/>
+    <mergeCell ref="F68:G68"/>
+    <mergeCell ref="F69:G69"/>
+    <mergeCell ref="F70:G70"/>
+    <mergeCell ref="A56:A58"/>
+    <mergeCell ref="B56:B58"/>
+    <mergeCell ref="F56:G56"/>
+    <mergeCell ref="F57:G57"/>
+    <mergeCell ref="F58:G58"/>
+    <mergeCell ref="A59:A61"/>
+    <mergeCell ref="B59:B61"/>
+    <mergeCell ref="F59:G59"/>
+    <mergeCell ref="F60:G60"/>
+    <mergeCell ref="F61:G61"/>
+    <mergeCell ref="F48:G48"/>
+    <mergeCell ref="F49:G49"/>
+    <mergeCell ref="A50:A55"/>
+    <mergeCell ref="B50:B55"/>
+    <mergeCell ref="F50:G50"/>
+    <mergeCell ref="F51:G51"/>
+    <mergeCell ref="F52:G52"/>
+    <mergeCell ref="F53:G53"/>
+    <mergeCell ref="F54:G54"/>
+    <mergeCell ref="F55:G55"/>
+    <mergeCell ref="F42:G42"/>
+    <mergeCell ref="A43:A47"/>
+    <mergeCell ref="B43:B47"/>
+    <mergeCell ref="F43:G43"/>
+    <mergeCell ref="F44:G44"/>
+    <mergeCell ref="F45:G45"/>
+    <mergeCell ref="F46:G46"/>
+    <mergeCell ref="F47:G47"/>
+    <mergeCell ref="A38:A41"/>
+    <mergeCell ref="B38:B41"/>
+    <mergeCell ref="F38:G38"/>
+    <mergeCell ref="F39:G39"/>
+    <mergeCell ref="F40:G40"/>
+    <mergeCell ref="F41:G41"/>
+    <mergeCell ref="A33:A37"/>
+    <mergeCell ref="B33:B37"/>
+    <mergeCell ref="F33:G33"/>
+    <mergeCell ref="F34:G34"/>
+    <mergeCell ref="F35:G35"/>
+    <mergeCell ref="F36:G36"/>
+    <mergeCell ref="F37:G37"/>
+    <mergeCell ref="A25:A32"/>
+    <mergeCell ref="B25:B32"/>
+    <mergeCell ref="F25:G25"/>
+    <mergeCell ref="F26:G26"/>
+    <mergeCell ref="F27:G27"/>
+    <mergeCell ref="F28:G28"/>
+    <mergeCell ref="F29:G29"/>
+    <mergeCell ref="F30:G30"/>
+    <mergeCell ref="F31:G31"/>
+    <mergeCell ref="F32:G32"/>
     <mergeCell ref="F19:G19"/>
     <mergeCell ref="F20:G20"/>
     <mergeCell ref="F21:G21"/>
@@ -4112,163 +4246,15 @@
     <mergeCell ref="F5:G5"/>
     <mergeCell ref="F6:G6"/>
     <mergeCell ref="F7:G7"/>
-    <mergeCell ref="A33:A37"/>
-    <mergeCell ref="B33:B37"/>
-    <mergeCell ref="F33:G33"/>
-    <mergeCell ref="F34:G34"/>
-    <mergeCell ref="F35:G35"/>
-    <mergeCell ref="F36:G36"/>
-    <mergeCell ref="F37:G37"/>
-    <mergeCell ref="A25:A32"/>
-    <mergeCell ref="B25:B32"/>
-    <mergeCell ref="F25:G25"/>
-    <mergeCell ref="F26:G26"/>
-    <mergeCell ref="F27:G27"/>
-    <mergeCell ref="F28:G28"/>
-    <mergeCell ref="F29:G29"/>
-    <mergeCell ref="F30:G30"/>
-    <mergeCell ref="F31:G31"/>
-    <mergeCell ref="F32:G32"/>
-    <mergeCell ref="F42:G42"/>
-    <mergeCell ref="A43:A47"/>
-    <mergeCell ref="B43:B47"/>
-    <mergeCell ref="F43:G43"/>
-    <mergeCell ref="F44:G44"/>
-    <mergeCell ref="F45:G45"/>
-    <mergeCell ref="F46:G46"/>
-    <mergeCell ref="F47:G47"/>
-    <mergeCell ref="A38:A41"/>
-    <mergeCell ref="B38:B41"/>
-    <mergeCell ref="F38:G38"/>
-    <mergeCell ref="F39:G39"/>
-    <mergeCell ref="F40:G40"/>
-    <mergeCell ref="F41:G41"/>
-    <mergeCell ref="F48:G48"/>
-    <mergeCell ref="F49:G49"/>
-    <mergeCell ref="A50:A55"/>
-    <mergeCell ref="B50:B55"/>
-    <mergeCell ref="F50:G50"/>
-    <mergeCell ref="F51:G51"/>
-    <mergeCell ref="F52:G52"/>
-    <mergeCell ref="F53:G53"/>
-    <mergeCell ref="F54:G54"/>
-    <mergeCell ref="F55:G55"/>
-    <mergeCell ref="A56:A58"/>
-    <mergeCell ref="B56:B58"/>
-    <mergeCell ref="F56:G56"/>
-    <mergeCell ref="F57:G57"/>
-    <mergeCell ref="F58:G58"/>
-    <mergeCell ref="A59:A61"/>
-    <mergeCell ref="B59:B61"/>
-    <mergeCell ref="F59:G59"/>
-    <mergeCell ref="F60:G60"/>
-    <mergeCell ref="F61:G61"/>
-    <mergeCell ref="A62:A64"/>
-    <mergeCell ref="B62:B64"/>
-    <mergeCell ref="F62:G62"/>
-    <mergeCell ref="F63:G63"/>
-    <mergeCell ref="F64:G64"/>
-    <mergeCell ref="A65:A70"/>
-    <mergeCell ref="B65:B70"/>
-    <mergeCell ref="F65:G65"/>
-    <mergeCell ref="F66:G66"/>
-    <mergeCell ref="F67:G67"/>
-    <mergeCell ref="F68:G68"/>
-    <mergeCell ref="F69:G69"/>
-    <mergeCell ref="F70:G70"/>
-    <mergeCell ref="A71:A75"/>
-    <mergeCell ref="B71:B75"/>
-    <mergeCell ref="F71:G71"/>
-    <mergeCell ref="F72:G72"/>
-    <mergeCell ref="F73:G73"/>
-    <mergeCell ref="F74:G74"/>
-    <mergeCell ref="F75:G75"/>
-    <mergeCell ref="A76:A78"/>
-    <mergeCell ref="B76:B78"/>
-    <mergeCell ref="F76:G76"/>
-    <mergeCell ref="F77:G77"/>
-    <mergeCell ref="F78:G78"/>
-    <mergeCell ref="A79:A81"/>
-    <mergeCell ref="B79:B81"/>
-    <mergeCell ref="F79:G79"/>
-    <mergeCell ref="F80:G80"/>
-    <mergeCell ref="F81:G81"/>
-    <mergeCell ref="A82:A84"/>
-    <mergeCell ref="B82:B84"/>
-    <mergeCell ref="F82:G82"/>
-    <mergeCell ref="F83:G83"/>
-    <mergeCell ref="F84:G84"/>
-    <mergeCell ref="A85:A90"/>
-    <mergeCell ref="B85:B90"/>
-    <mergeCell ref="F85:G85"/>
-    <mergeCell ref="F86:G86"/>
-    <mergeCell ref="F87:G87"/>
-    <mergeCell ref="F88:G88"/>
-    <mergeCell ref="F89:G89"/>
-    <mergeCell ref="F90:G90"/>
-    <mergeCell ref="F91:G91"/>
-    <mergeCell ref="A92:A95"/>
-    <mergeCell ref="B92:B95"/>
-    <mergeCell ref="F92:G92"/>
-    <mergeCell ref="F93:G93"/>
-    <mergeCell ref="F94:G94"/>
-    <mergeCell ref="F95:G95"/>
-    <mergeCell ref="A100:A103"/>
-    <mergeCell ref="B100:B103"/>
-    <mergeCell ref="F100:G100"/>
-    <mergeCell ref="F101:G101"/>
-    <mergeCell ref="F102:G102"/>
-    <mergeCell ref="F103:G103"/>
-    <mergeCell ref="A96:A99"/>
-    <mergeCell ref="B96:B99"/>
-    <mergeCell ref="F96:G96"/>
-    <mergeCell ref="F97:G97"/>
-    <mergeCell ref="F98:G98"/>
-    <mergeCell ref="F99:G99"/>
-    <mergeCell ref="A104:A105"/>
-    <mergeCell ref="B104:B105"/>
-    <mergeCell ref="F104:G104"/>
-    <mergeCell ref="F105:G105"/>
-    <mergeCell ref="A106:A114"/>
-    <mergeCell ref="B106:B114"/>
-    <mergeCell ref="F106:G106"/>
-    <mergeCell ref="F107:G107"/>
-    <mergeCell ref="F108:G108"/>
-    <mergeCell ref="F109:G109"/>
-    <mergeCell ref="A117:A118"/>
-    <mergeCell ref="B117:B118"/>
-    <mergeCell ref="F117:G117"/>
-    <mergeCell ref="F118:G118"/>
-    <mergeCell ref="F110:G110"/>
-    <mergeCell ref="F111:G111"/>
-    <mergeCell ref="F112:G112"/>
-    <mergeCell ref="F113:G113"/>
-    <mergeCell ref="F114:G114"/>
-    <mergeCell ref="A115:A116"/>
-    <mergeCell ref="B115:B116"/>
-    <mergeCell ref="F115:G115"/>
-    <mergeCell ref="F116:G116"/>
-    <mergeCell ref="B121:B125"/>
-    <mergeCell ref="F121:G121"/>
-    <mergeCell ref="F122:G122"/>
-    <mergeCell ref="F123:G123"/>
-    <mergeCell ref="A135:H135"/>
-    <mergeCell ref="F131:G131"/>
-    <mergeCell ref="A132:A134"/>
-    <mergeCell ref="B132:B134"/>
-    <mergeCell ref="F132:G132"/>
-    <mergeCell ref="F133:G133"/>
-    <mergeCell ref="F134:G134"/>
-    <mergeCell ref="F124:G124"/>
-    <mergeCell ref="F125:G125"/>
-    <mergeCell ref="A126:A130"/>
-    <mergeCell ref="B126:B130"/>
-    <mergeCell ref="F126:G126"/>
-    <mergeCell ref="F127:G127"/>
-    <mergeCell ref="F128:G128"/>
-    <mergeCell ref="F129:G129"/>
-    <mergeCell ref="F130:G130"/>
-    <mergeCell ref="A121:A125"/>
+    <mergeCell ref="F8:G8"/>
+    <mergeCell ref="F9:G9"/>
+    <mergeCell ref="F10:G10"/>
+    <mergeCell ref="A1:A2"/>
+    <mergeCell ref="B1:B2"/>
+    <mergeCell ref="C1:C2"/>
+    <mergeCell ref="D1:D2"/>
+    <mergeCell ref="E1:H1"/>
+    <mergeCell ref="F2:G2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>

</xml_diff>